<commit_message>
Update NI_vannf with the changes implemented in WFD2ECA
</commit_message>
<xml_diff>
--- a/data/VM-param.xlsx
+++ b/data/VM-param.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\nina\NatInd\2023\klassegr\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\hanno.sandvik\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{81849DFE-0F23-40E0-B844-3FFD0A388BD3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{61A11C51-AB85-4F1C-8F74-0A2246479207}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="VM-param" sheetId="1" r:id="rId1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1312" uniqueCount="680">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1296" uniqueCount="681">
   <si>
     <t>id</t>
   </si>
@@ -2073,6 +2073,9 @@
   </si>
   <si>
     <t>Trusselgrad</t>
+  </si>
+  <si>
+    <t>Inf</t>
   </si>
 </sst>
 </file>
@@ -2617,9 +2620,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -2657,7 +2660,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -2763,7 +2766,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -2905,7 +2908,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -2915,7 +2918,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D340"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A258" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A298" workbookViewId="0">
       <selection activeCell="D334" sqref="D334"/>
     </sheetView>
   </sheetViews>
@@ -3138,11 +3141,11 @@
       <c r="B16" t="s">
         <v>34</v>
       </c>
-      <c r="C16" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" t="s">
-        <v>6</v>
+      <c r="C16">
+        <v>-200</v>
+      </c>
+      <c r="D16">
+        <v>250</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.25">
@@ -5112,11 +5115,11 @@
       <c r="B157" t="s">
         <v>313</v>
       </c>
-      <c r="C157" t="s">
-        <v>6</v>
+      <c r="C157">
+        <v>0</v>
       </c>
       <c r="D157" t="s">
-        <v>6</v>
+        <v>680</v>
       </c>
     </row>
     <row r="158" spans="1:4" x14ac:dyDescent="0.25">
@@ -5238,11 +5241,11 @@
       <c r="B166" t="s">
         <v>331</v>
       </c>
-      <c r="C166" t="s">
-        <v>6</v>
+      <c r="C166">
+        <v>0</v>
       </c>
       <c r="D166" t="s">
-        <v>6</v>
+        <v>680</v>
       </c>
     </row>
     <row r="167" spans="1:4" x14ac:dyDescent="0.25">
@@ -6526,11 +6529,11 @@
       <c r="B258" t="s">
         <v>515</v>
       </c>
-      <c r="C258" t="s">
-        <v>6</v>
-      </c>
-      <c r="D258" t="s">
-        <v>6</v>
+      <c r="C258">
+        <v>0</v>
+      </c>
+      <c r="D258">
+        <v>1000000</v>
       </c>
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
@@ -6694,11 +6697,11 @@
       <c r="B270" t="s">
         <v>539</v>
       </c>
-      <c r="C270" t="s">
-        <v>6</v>
+      <c r="C270">
+        <v>0</v>
       </c>
       <c r="D270" t="s">
-        <v>6</v>
+        <v>680</v>
       </c>
     </row>
     <row r="271" spans="1:4" x14ac:dyDescent="0.25">
@@ -6806,11 +6809,11 @@
       <c r="B278" t="s">
         <v>555</v>
       </c>
-      <c r="C278" t="s">
-        <v>6</v>
-      </c>
-      <c r="D278" t="s">
-        <v>6</v>
+      <c r="C278">
+        <v>3.2</v>
+      </c>
+      <c r="D278">
+        <v>10.8</v>
       </c>
     </row>
     <row r="279" spans="1:4" x14ac:dyDescent="0.25">
@@ -7128,11 +7131,11 @@
       <c r="B301" t="s">
         <v>601</v>
       </c>
-      <c r="C301" t="s">
-        <v>6</v>
+      <c r="C301">
+        <v>0</v>
       </c>
       <c r="D301" t="s">
-        <v>6</v>
+        <v>680</v>
       </c>
     </row>
     <row r="302" spans="1:4" x14ac:dyDescent="0.25">
@@ -7212,11 +7215,11 @@
       <c r="B307" t="s">
         <v>613</v>
       </c>
-      <c r="C307" t="s">
-        <v>6</v>
-      </c>
-      <c r="D307" t="s">
-        <v>6</v>
+      <c r="C307">
+        <v>2</v>
+      </c>
+      <c r="D307">
+        <v>8</v>
       </c>
     </row>
     <row r="308" spans="1:4" x14ac:dyDescent="0.25">
@@ -7324,11 +7327,11 @@
       <c r="B315" t="s">
         <v>629</v>
       </c>
-      <c r="C315" t="s">
-        <v>6</v>
-      </c>
-      <c r="D315" t="s">
-        <v>6</v>
+      <c r="C315">
+        <v>0</v>
+      </c>
+      <c r="D315">
+        <v>60</v>
       </c>
     </row>
     <row r="316" spans="1:4" x14ac:dyDescent="0.25">
@@ -7548,11 +7551,11 @@
       <c r="B331" t="s">
         <v>661</v>
       </c>
-      <c r="C331" t="s">
-        <v>6</v>
-      </c>
-      <c r="D331" t="s">
-        <v>6</v>
+      <c r="C331">
+        <v>0</v>
+      </c>
+      <c r="D331">
+        <v>150</v>
       </c>
     </row>
     <row r="332" spans="1:4" x14ac:dyDescent="0.25">

</xml_diff>